<commit_message>
Demo Build with end to end complete
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/CanineDatafromNeo4j_1.xlsx
+++ b/CTDC_Automation/TestData/CanineDatafromNeo4j_1.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\DemoBuild\DataCommons_Automation\CTDC_Automation\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D49B31-CECC-4153-B2E5-C698613B8973}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView minimized="1" xWindow="8610" yWindow="3450" windowWidth="12225" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CypherOutput" r:id="rId3" sheetId="1"/>
-    <sheet name="Message" r:id="rId4" sheetId="2"/>
+    <sheet name="CypherOutput" sheetId="1" r:id="rId1"/>
+    <sheet name="Message" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="298">
   <si>
     <t>Case ID</t>
   </si>
@@ -408,9 +416,6 @@
     <t>4.2</t>
   </si>
   <si>
-    <t>COTC007B0101</t>
-  </si>
-  <si>
     <t>10.1</t>
   </si>
   <si>
@@ -898,16 +903,27 @@
   </si>
   <si>
     <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\CanineDatafromNeo4j.xlsx</t>
+  </si>
+  <si>
+    <t>COTC007B0101_laxmi</t>
+  </si>
+  <si>
+    <t>COTC007B_Laxmi</t>
+  </si>
+  <si>
+    <t>III_laxmi</t>
+  </si>
+  <si>
+    <t>Male Phenotype_laxmi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -919,7 +935,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -937,18 +953,333 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I145"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +1305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +1331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1026,7 +1357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1052,7 +1383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1078,7 +1409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1104,7 +1435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1130,7 +1461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1156,7 +1487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1182,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1208,7 +1539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1234,7 +1565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1260,7 +1591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1286,7 +1617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1312,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1338,7 +1669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1364,7 +1695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1390,7 +1721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1416,7 +1747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1442,7 +1773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1468,7 +1799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1494,7 +1825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1520,7 +1851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1546,7 +1877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1572,7 +1903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1598,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -1624,7 +1955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1650,7 +1981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -1676,7 +2007,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1702,7 +2033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1728,7 +2059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -1754,7 +2085,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1780,7 +2111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -1806,7 +2137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1832,7 +2163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -1858,7 +2189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -1884,7 +2215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -1910,7 +2241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1936,7 +2267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1962,7 +2293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1988,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -2014,7 +2345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -2040,7 +2371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>95</v>
       </c>
@@ -2066,7 +2397,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -2092,7 +2423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -2118,7 +2449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2144,7 +2475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>102</v>
       </c>
@@ -2170,7 +2501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -2196,7 +2527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -2222,7 +2553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -2248,7 +2579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -2274,7 +2605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -2300,7 +2631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -2326,7 +2657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -2352,7 +2683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -2378,7 +2709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -2404,7 +2735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2430,7 +2761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -2456,7 +2787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -2482,7 +2813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -2508,7 +2839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -2534,7 +2865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -2560,7 +2891,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -2586,9 +2917,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>294</v>
       </c>
       <c r="B64" t="s">
         <v>124</v>
@@ -2606,41 +2937,41 @@
         <v>127</v>
       </c>
       <c r="G64" t="s">
+        <v>131</v>
+      </c>
+      <c r="H64" t="s">
         <v>132</v>
       </c>
-      <c r="H64" t="s">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" t="s">
         <v>134</v>
-      </c>
-      <c r="B65" t="s">
-        <v>124</v>
-      </c>
-      <c r="C65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D65" t="s">
-        <v>135</v>
       </c>
       <c r="E65" t="s">
         <v>126</v>
       </c>
       <c r="F65" t="s">
+        <v>135</v>
+      </c>
+      <c r="G65" t="s">
         <v>136</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>137</v>
       </c>
-      <c r="H65" t="s">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>139</v>
       </c>
       <c r="B66" t="s">
         <v>124</v>
@@ -2652,44 +2983,44 @@
         <v>11</v>
       </c>
       <c r="E66" t="s">
+        <v>139</v>
+      </c>
+      <c r="F66" t="s">
         <v>140</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>141</v>
       </c>
-      <c r="G66" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" t="s">
         <v>142</v>
       </c>
-      <c r="B67" t="s">
-        <v>124</v>
-      </c>
-      <c r="C67" t="s">
-        <v>125</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>143</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>144</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>145</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>146</v>
       </c>
-      <c r="H67" t="s">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>148</v>
       </c>
       <c r="B68" t="s">
         <v>124</v>
@@ -2713,12 +3044,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>295</v>
       </c>
       <c r="C69" t="s">
         <v>125</v>
@@ -2727,21 +3058,21 @@
         <v>29</v>
       </c>
       <c r="E69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F69" t="s">
-        <v>136</v>
+        <v>296</v>
       </c>
       <c r="G69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>150</v>
-      </c>
-      <c r="H69" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>151</v>
       </c>
       <c r="B70" t="s">
         <v>124</v>
@@ -2753,21 +3084,21 @@
         <v>54</v>
       </c>
       <c r="E70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" t="s">
         <v>152</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>153</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>154</v>
-      </c>
-      <c r="H70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>155</v>
       </c>
       <c r="B71" t="s">
         <v>124</v>
@@ -2779,10 +3110,10 @@
         <v>11</v>
       </c>
       <c r="E71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G71" t="s">
         <v>24</v>
@@ -2791,9 +3122,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B72" t="s">
         <v>124</v>
@@ -2805,21 +3136,21 @@
         <v>31</v>
       </c>
       <c r="E72" t="s">
+        <v>156</v>
+      </c>
+      <c r="F72" t="s">
+        <v>156</v>
+      </c>
+      <c r="G72" t="s">
         <v>157</v>
-      </c>
-      <c r="F72" t="s">
-        <v>157</v>
-      </c>
-      <c r="G72" t="s">
-        <v>158</v>
       </c>
       <c r="H72" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
         <v>124</v>
@@ -2831,48 +3162,48 @@
         <v>42</v>
       </c>
       <c r="E73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F73" t="s">
         <v>127</v>
       </c>
       <c r="G73" t="s">
+        <v>160</v>
+      </c>
+      <c r="H73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>161</v>
       </c>
-      <c r="H73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" t="s">
         <v>162</v>
-      </c>
-      <c r="B74" t="s">
-        <v>124</v>
-      </c>
-      <c r="C74" t="s">
-        <v>125</v>
-      </c>
-      <c r="D74" t="s">
-        <v>163</v>
       </c>
       <c r="E74" t="s">
         <v>126</v>
       </c>
       <c r="F74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G74" t="s">
+        <v>163</v>
+      </c>
+      <c r="H74" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>164</v>
       </c>
-      <c r="H74" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>165</v>
-      </c>
       <c r="B75" t="s">
         <v>124</v>
       </c>
@@ -2880,7 +3211,7 @@
         <v>125</v>
       </c>
       <c r="D75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E75" t="s">
         <v>126</v>
@@ -2889,15 +3220,15 @@
         <v>127</v>
       </c>
       <c r="G75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H75" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
         <v>124</v>
@@ -2915,15 +3246,15 @@
         <v>127</v>
       </c>
       <c r="G76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H76" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B77" t="s">
         <v>124</v>
@@ -2935,10 +3266,10 @@
         <v>31</v>
       </c>
       <c r="E77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G77" t="s">
         <v>24</v>
@@ -2947,35 +3278,35 @@
         <v>128</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" t="s">
         <v>171</v>
       </c>
-      <c r="B78" t="s">
-        <v>124</v>
-      </c>
-      <c r="C78" t="s">
-        <v>125</v>
-      </c>
-      <c r="D78" t="s">
-        <v>172</v>
-      </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F78" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G78" t="s">
         <v>24</v>
       </c>
       <c r="H78" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
         <v>124</v>
@@ -2984,7 +3315,7 @@
         <v>125</v>
       </c>
       <c r="D79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E79" t="s">
         <v>126</v>
@@ -2993,41 +3324,41 @@
         <v>127</v>
       </c>
       <c r="G79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H79" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>174</v>
+      </c>
+      <c r="B80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" t="s">
+        <v>125</v>
+      </c>
+      <c r="D80" t="s">
         <v>175</v>
-      </c>
-      <c r="B80" t="s">
-        <v>124</v>
-      </c>
-      <c r="C80" t="s">
-        <v>125</v>
-      </c>
-      <c r="D80" t="s">
-        <v>176</v>
       </c>
       <c r="E80" t="s">
         <v>126</v>
       </c>
       <c r="F80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G80" t="s">
         <v>130</v>
       </c>
       <c r="H80" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B81" t="s">
         <v>124</v>
@@ -3045,15 +3376,15 @@
         <v>127</v>
       </c>
       <c r="G81" t="s">
+        <v>177</v>
+      </c>
+      <c r="H81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>178</v>
-      </c>
-      <c r="H81" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>179</v>
       </c>
       <c r="B82" t="s">
         <v>124</v>
@@ -3065,18 +3396,18 @@
         <v>86</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F82" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G82" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B83" t="s">
         <v>124</v>
@@ -3094,15 +3425,15 @@
         <v>127</v>
       </c>
       <c r="G83" t="s">
+        <v>180</v>
+      </c>
+      <c r="H83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>181</v>
-      </c>
-      <c r="H83" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>182</v>
       </c>
       <c r="B84" t="s">
         <v>124</v>
@@ -3120,15 +3451,15 @@
         <v>127</v>
       </c>
       <c r="G84" t="s">
+        <v>182</v>
+      </c>
+      <c r="H84" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>183</v>
-      </c>
-      <c r="H84" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>184</v>
       </c>
       <c r="B85" t="s">
         <v>124</v>
@@ -3140,10 +3471,10 @@
         <v>103</v>
       </c>
       <c r="E85" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F85" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G85" t="s">
         <v>24</v>
@@ -3152,18 +3483,18 @@
         <v>128</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" t="s">
+        <v>125</v>
+      </c>
+      <c r="D86" t="s">
         <v>185</v>
-      </c>
-      <c r="B86" t="s">
-        <v>124</v>
-      </c>
-      <c r="C86" t="s">
-        <v>125</v>
-      </c>
-      <c r="D86" t="s">
-        <v>186</v>
       </c>
       <c r="E86" t="s">
         <v>126</v>
@@ -3175,12 +3506,12 @@
         <v>71</v>
       </c>
       <c r="H86" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B87" t="s">
         <v>124</v>
@@ -3198,15 +3529,15 @@
         <v>127</v>
       </c>
       <c r="G87" t="s">
+        <v>187</v>
+      </c>
+      <c r="H87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>188</v>
-      </c>
-      <c r="H87" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>189</v>
       </c>
       <c r="B88" t="s">
         <v>124</v>
@@ -3218,18 +3549,18 @@
         <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G88" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B89" t="s">
         <v>124</v>
@@ -3244,18 +3575,18 @@
         <v>126</v>
       </c>
       <c r="F89" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H89" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
         <v>124</v>
@@ -3276,9 +3607,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
         <v>124</v>
@@ -3290,21 +3621,21 @@
         <v>31</v>
       </c>
       <c r="E91" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G91" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H91" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B92" t="s">
         <v>124</v>
@@ -3316,27 +3647,27 @@
         <v>47</v>
       </c>
       <c r="E92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F92" t="s">
         <v>127</v>
       </c>
       <c r="G92" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>194</v>
+      </c>
+      <c r="B93" t="s">
+        <v>124</v>
+      </c>
+      <c r="C93" t="s">
+        <v>125</v>
+      </c>
+      <c r="D93" t="s">
         <v>195</v>
-      </c>
-      <c r="B93" t="s">
-        <v>124</v>
-      </c>
-      <c r="C93" t="s">
-        <v>125</v>
-      </c>
-      <c r="D93" t="s">
-        <v>196</v>
       </c>
       <c r="E93" t="s">
         <v>126</v>
@@ -3345,15 +3676,15 @@
         <v>127</v>
       </c>
       <c r="G93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H93" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B94" t="s">
         <v>124</v>
@@ -3365,10 +3696,10 @@
         <v>120</v>
       </c>
       <c r="E94" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" t="s">
         <v>144</v>
-      </c>
-      <c r="F94" t="s">
-        <v>145</v>
       </c>
       <c r="G94" t="s">
         <v>130</v>
@@ -3377,9 +3708,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B95" t="s">
         <v>124</v>
@@ -3391,18 +3722,18 @@
         <v>62</v>
       </c>
       <c r="E95" t="s">
+        <v>199</v>
+      </c>
+      <c r="F95" t="s">
+        <v>144</v>
+      </c>
+      <c r="G95" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>200</v>
-      </c>
-      <c r="F95" t="s">
-        <v>145</v>
-      </c>
-      <c r="G95" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>201</v>
       </c>
       <c r="B96" t="s">
         <v>124</v>
@@ -3420,24 +3751,24 @@
         <v>127</v>
       </c>
       <c r="G96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H96" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>202</v>
+      </c>
+      <c r="B97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" t="s">
         <v>203</v>
-      </c>
-      <c r="B97" t="s">
-        <v>124</v>
-      </c>
-      <c r="C97" t="s">
-        <v>125</v>
-      </c>
-      <c r="D97" t="s">
-        <v>204</v>
       </c>
       <c r="E97" t="s">
         <v>126</v>
@@ -3446,41 +3777,41 @@
         <v>127</v>
       </c>
       <c r="G97" t="s">
+        <v>204</v>
+      </c>
+      <c r="H97" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>205</v>
       </c>
-      <c r="H97" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
+        <v>124</v>
+      </c>
+      <c r="C98" t="s">
+        <v>125</v>
+      </c>
+      <c r="D98" t="s">
         <v>206</v>
       </c>
-      <c r="B98" t="s">
-        <v>124</v>
-      </c>
-      <c r="C98" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" t="s">
-        <v>207</v>
-      </c>
       <c r="E98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F98" t="s">
         <v>127</v>
       </c>
       <c r="G98" t="s">
+        <v>207</v>
+      </c>
+      <c r="H98" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>208</v>
-      </c>
-      <c r="H98" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>209</v>
       </c>
       <c r="B99" t="s">
         <v>124</v>
@@ -3501,24 +3832,24 @@
         <v>128</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100" t="s">
+        <v>125</v>
+      </c>
+      <c r="D100" t="s">
+        <v>195</v>
+      </c>
+      <c r="E100" t="s">
+        <v>143</v>
+      </c>
+      <c r="F100" t="s">
         <v>210</v>
-      </c>
-      <c r="B100" t="s">
-        <v>124</v>
-      </c>
-      <c r="C100" t="s">
-        <v>125</v>
-      </c>
-      <c r="D100" t="s">
-        <v>196</v>
-      </c>
-      <c r="E100" t="s">
-        <v>144</v>
-      </c>
-      <c r="F100" t="s">
-        <v>211</v>
       </c>
       <c r="G100" t="s">
         <v>66</v>
@@ -3527,9 +3858,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B101" t="s">
         <v>124</v>
@@ -3547,15 +3878,15 @@
         <v>127</v>
       </c>
       <c r="G101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H101" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B102" t="s">
         <v>124</v>
@@ -3570,18 +3901,18 @@
         <v>126</v>
       </c>
       <c r="F102" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G102" t="s">
+        <v>214</v>
+      </c>
+      <c r="H102" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>215</v>
-      </c>
-      <c r="H102" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
-        <v>216</v>
       </c>
       <c r="B103" t="s">
         <v>124</v>
@@ -3602,12 +3933,12 @@
         <v>19</v>
       </c>
       <c r="H103" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B104" t="s">
         <v>124</v>
@@ -3619,21 +3950,21 @@
         <v>11</v>
       </c>
       <c r="E104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F104" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H104" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B105" t="s">
         <v>124</v>
@@ -3645,21 +3976,21 @@
         <v>86</v>
       </c>
       <c r="E105" t="s">
+        <v>219</v>
+      </c>
+      <c r="F105" t="s">
         <v>220</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
+        <v>131</v>
+      </c>
+      <c r="H105" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>221</v>
-      </c>
-      <c r="G105" t="s">
-        <v>132</v>
-      </c>
-      <c r="H105" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>222</v>
       </c>
       <c r="B106" t="s">
         <v>124</v>
@@ -3671,21 +4002,21 @@
         <v>11</v>
       </c>
       <c r="E106" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F106" t="s">
+        <v>222</v>
+      </c>
+      <c r="G106" t="s">
         <v>223</v>
-      </c>
-      <c r="G106" t="s">
-        <v>224</v>
       </c>
       <c r="H106" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B107" t="s">
         <v>124</v>
@@ -3697,21 +4028,21 @@
         <v>96</v>
       </c>
       <c r="E107" t="s">
+        <v>151</v>
+      </c>
+      <c r="F107" t="s">
         <v>152</v>
       </c>
-      <c r="F107" t="s">
-        <v>153</v>
-      </c>
       <c r="G107" t="s">
+        <v>225</v>
+      </c>
+      <c r="H107" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>226</v>
-      </c>
-      <c r="H107" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s">
-        <v>227</v>
       </c>
       <c r="B108" t="s">
         <v>124</v>
@@ -3729,15 +4060,15 @@
         <v>127</v>
       </c>
       <c r="G108" t="s">
+        <v>227</v>
+      </c>
+      <c r="H108" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>228</v>
-      </c>
-      <c r="H108" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>229</v>
       </c>
       <c r="B109" t="s">
         <v>124</v>
@@ -3755,15 +4086,15 @@
         <v>127</v>
       </c>
       <c r="G109" t="s">
+        <v>229</v>
+      </c>
+      <c r="H109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>230</v>
-      </c>
-      <c r="H109" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s">
-        <v>231</v>
       </c>
       <c r="B110" t="s">
         <v>124</v>
@@ -3775,21 +4106,21 @@
         <v>86</v>
       </c>
       <c r="E110" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H110" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B111" t="s">
         <v>124</v>
@@ -3801,21 +4132,21 @@
         <v>11</v>
       </c>
       <c r="E111" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F111" t="s">
         <v>127</v>
       </c>
       <c r="G111" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H111" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B112" t="s">
         <v>124</v>
@@ -3830,18 +4161,18 @@
         <v>126</v>
       </c>
       <c r="F112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G112" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H112" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B113" t="s">
         <v>124</v>
@@ -3850,24 +4181,24 @@
         <v>125</v>
       </c>
       <c r="D113" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E113" t="s">
         <v>126</v>
       </c>
       <c r="F113" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G113" t="s">
         <v>40</v>
       </c>
       <c r="H113" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B114" t="s">
         <v>124</v>
@@ -3879,30 +4210,30 @@
         <v>62</v>
       </c>
       <c r="E114" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F114" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H114" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="115">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>235</v>
+      </c>
+      <c r="B115" t="s">
+        <v>124</v>
+      </c>
+      <c r="C115" t="s">
+        <v>125</v>
+      </c>
+      <c r="D115" t="s">
         <v>236</v>
-      </c>
-      <c r="B115" t="s">
-        <v>124</v>
-      </c>
-      <c r="C115" t="s">
-        <v>125</v>
-      </c>
-      <c r="D115" t="s">
-        <v>237</v>
       </c>
       <c r="E115" t="s">
         <v>126</v>
@@ -3911,15 +4242,15 @@
         <v>127</v>
       </c>
       <c r="G115" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H115" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B116" t="s">
         <v>124</v>
@@ -3931,21 +4262,21 @@
         <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G116" t="s">
         <v>27</v>
       </c>
       <c r="H116" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="117">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B117" t="s">
         <v>124</v>
@@ -3957,21 +4288,21 @@
         <v>39</v>
       </c>
       <c r="E117" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F117" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G117" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H117" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B118" t="s">
         <v>124</v>
@@ -3983,7 +4314,7 @@
         <v>31</v>
       </c>
       <c r="E118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F118" t="s">
         <v>127</v>
@@ -3992,9 +4323,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B119" t="s">
         <v>124</v>
@@ -4006,10 +4337,10 @@
         <v>31</v>
       </c>
       <c r="E119" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F119" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G119" t="s">
         <v>13</v>
@@ -4018,9 +4349,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B120" t="s">
         <v>124</v>
@@ -4035,18 +4366,18 @@
         <v>126</v>
       </c>
       <c r="F120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H120" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B121" t="s">
         <v>124</v>
@@ -4061,18 +4392,18 @@
         <v>126</v>
       </c>
       <c r="F121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H121" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B122" t="s">
         <v>124</v>
@@ -4084,21 +4415,21 @@
         <v>42</v>
       </c>
       <c r="E122" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F122" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H122" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B123" t="s">
         <v>124</v>
@@ -4110,21 +4441,21 @@
         <v>31</v>
       </c>
       <c r="E123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F123" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G123" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H123" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="124">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B124" t="s">
         <v>124</v>
@@ -4145,9 +4476,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
         <v>124</v>
@@ -4168,12 +4499,12 @@
         <v>24</v>
       </c>
       <c r="H125" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="126">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B126" t="s">
         <v>124</v>
@@ -4185,21 +4516,21 @@
         <v>11</v>
       </c>
       <c r="E126" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G126" t="s">
+        <v>253</v>
+      </c>
+      <c r="H126" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>254</v>
-      </c>
-      <c r="H126" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>255</v>
       </c>
       <c r="B127" t="s">
         <v>124</v>
@@ -4217,15 +4548,15 @@
         <v>127</v>
       </c>
       <c r="G127" t="s">
+        <v>255</v>
+      </c>
+      <c r="H127" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>256</v>
-      </c>
-      <c r="H127" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
-        <v>257</v>
       </c>
       <c r="B128" t="s">
         <v>124</v>
@@ -4246,9 +4577,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B129" t="s">
         <v>124</v>
@@ -4260,21 +4591,21 @@
         <v>86</v>
       </c>
       <c r="E129" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G129" t="s">
+        <v>258</v>
+      </c>
+      <c r="H129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>259</v>
-      </c>
-      <c r="H129" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s">
-        <v>260</v>
       </c>
       <c r="B130" t="s">
         <v>124</v>
@@ -4286,18 +4617,18 @@
         <v>31</v>
       </c>
       <c r="E130" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F130" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G130" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="131">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B131" t="s">
         <v>124</v>
@@ -4309,18 +4640,18 @@
         <v>54</v>
       </c>
       <c r="E131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F131" t="s">
         <v>127</v>
       </c>
       <c r="G131" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="132">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B132" t="s">
         <v>124</v>
@@ -4338,41 +4669,41 @@
         <v>127</v>
       </c>
       <c r="G132" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H132" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>263</v>
+      </c>
+      <c r="B133" t="s">
+        <v>124</v>
+      </c>
+      <c r="C133" t="s">
+        <v>125</v>
+      </c>
+      <c r="D133" t="s">
+        <v>142</v>
+      </c>
+      <c r="E133" t="s">
+        <v>199</v>
+      </c>
+      <c r="F133" t="s">
+        <v>144</v>
+      </c>
+      <c r="G133" t="s">
+        <v>253</v>
+      </c>
+      <c r="H133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>264</v>
-      </c>
-      <c r="B133" t="s">
-        <v>124</v>
-      </c>
-      <c r="C133" t="s">
-        <v>125</v>
-      </c>
-      <c r="D133" t="s">
-        <v>143</v>
-      </c>
-      <c r="E133" t="s">
-        <v>200</v>
-      </c>
-      <c r="F133" t="s">
-        <v>145</v>
-      </c>
-      <c r="G133" t="s">
-        <v>254</v>
-      </c>
-      <c r="H133" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="s">
-        <v>265</v>
       </c>
       <c r="B134" t="s">
         <v>124</v>
@@ -4384,21 +4715,21 @@
         <v>54</v>
       </c>
       <c r="E134" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F134" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G134" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H134" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="135">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B135" t="s">
         <v>124</v>
@@ -4410,21 +4741,21 @@
         <v>29</v>
       </c>
       <c r="E135" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F135" t="s">
         <v>127</v>
       </c>
       <c r="G135" t="s">
+        <v>266</v>
+      </c>
+      <c r="H135" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>267</v>
-      </c>
-      <c r="H135" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="s">
-        <v>268</v>
       </c>
       <c r="B136" t="s">
         <v>124</v>
@@ -4436,21 +4767,21 @@
         <v>11</v>
       </c>
       <c r="E136" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F136" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G136" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H136" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="137">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B137" t="s">
         <v>124</v>
@@ -4462,21 +4793,21 @@
         <v>31</v>
       </c>
       <c r="E137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G137" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H137" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="138">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B138" t="s">
         <v>124</v>
@@ -4491,44 +4822,44 @@
         <v>126</v>
       </c>
       <c r="F138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G138" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>270</v>
+      </c>
+      <c r="B139" t="s">
+        <v>124</v>
+      </c>
+      <c r="C139" t="s">
+        <v>125</v>
+      </c>
+      <c r="D139" t="s">
         <v>271</v>
       </c>
-      <c r="B139" t="s">
-        <v>124</v>
-      </c>
-      <c r="C139" t="s">
-        <v>125</v>
-      </c>
-      <c r="D139" t="s">
+      <c r="E139" t="s">
+        <v>139</v>
+      </c>
+      <c r="F139" t="s">
+        <v>135</v>
+      </c>
+      <c r="G139" t="s">
         <v>272</v>
-      </c>
-      <c r="E139" t="s">
-        <v>140</v>
-      </c>
-      <c r="F139" t="s">
-        <v>136</v>
-      </c>
-      <c r="G139" t="s">
-        <v>273</v>
       </c>
       <c r="H139" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B140" t="s">
         <v>124</v>
@@ -4546,38 +4877,38 @@
         <v>127</v>
       </c>
       <c r="G140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H140" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>274</v>
+      </c>
+      <c r="B141" t="s">
+        <v>124</v>
+      </c>
+      <c r="C141" t="s">
+        <v>125</v>
+      </c>
+      <c r="D141" t="s">
         <v>275</v>
       </c>
-      <c r="B141" t="s">
-        <v>124</v>
-      </c>
-      <c r="C141" t="s">
-        <v>125</v>
-      </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
+        <v>143</v>
+      </c>
+      <c r="F141" t="s">
+        <v>144</v>
+      </c>
+      <c r="G141" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>276</v>
-      </c>
-      <c r="E141" t="s">
-        <v>144</v>
-      </c>
-      <c r="F141" t="s">
-        <v>145</v>
-      </c>
-      <c r="G141" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="s">
-        <v>277</v>
       </c>
       <c r="B142" t="s">
         <v>124</v>
@@ -4589,21 +4920,21 @@
         <v>11</v>
       </c>
       <c r="E142" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F142" t="s">
         <v>127</v>
       </c>
       <c r="G142" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H142" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B143" t="s">
         <v>124</v>
@@ -4615,21 +4946,21 @@
         <v>22</v>
       </c>
       <c r="E143" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F143" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G143" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H143" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B144" t="s">
         <v>124</v>
@@ -4641,21 +4972,21 @@
         <v>11</v>
       </c>
       <c r="E144" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G144" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H144" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B145" t="s">
         <v>124</v>
@@ -4667,82 +4998,82 @@
         <v>62</v>
       </c>
       <c r="E145" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F145" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G145" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H145" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>294</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>